<commit_message>
Commented out prints, and added germ to content buckets
</commit_message>
<xml_diff>
--- a/Content Buckets.xlsx
+++ b/Content Buckets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="754">
   <si>
     <t>Lexical item</t>
   </si>
@@ -917,6 +917,9 @@
   </si>
   <si>
     <t>disease</t>
+  </si>
+  <si>
+    <t>germ</t>
   </si>
   <si>
     <t>pandemic</t>
@@ -5869,27 +5872,24 @@
         <v>311</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="C306" s="1">
         <v>-1.0</v>
-      </c>
-      <c r="D306" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C307" s="1">
+        <v>-1.0</v>
+      </c>
+      <c r="D307" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="B307" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C307" s="1">
-        <v>-1.0</v>
-      </c>
-      <c r="D307" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="308">
@@ -5897,13 +5897,13 @@
         <v>315</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C308" s="1">
         <v>-1.0</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="309">
@@ -5911,27 +5911,27 @@
         <v>316</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C309" s="1">
-        <v>1.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C310" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D310" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C310" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D310" s="1" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="311">
@@ -5939,13 +5939,13 @@
         <v>320</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C311" s="1">
         <v>1.0</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="312">
@@ -5953,13 +5953,13 @@
         <v>321</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C312" s="1">
         <v>1.0</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="313">
@@ -5967,13 +5967,13 @@
         <v>322</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C313" s="1">
         <v>1.0</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="314">
@@ -5981,27 +5981,27 @@
         <v>323</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="C314" s="1">
         <v>1.0</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C315" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D315" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="B315" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="C315" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D315" s="1" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="316">
@@ -6009,13 +6009,13 @@
         <v>327</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C316" s="1">
         <v>1.0</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="317">
@@ -6023,13 +6023,13 @@
         <v>328</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C317" s="1">
         <v>1.0</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="318">
@@ -6037,13 +6037,13 @@
         <v>329</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C318" s="1">
         <v>1.0</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="319">
@@ -6051,13 +6051,13 @@
         <v>330</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C319" s="1">
         <v>1.0</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="320">
@@ -6065,13 +6065,13 @@
         <v>331</v>
       </c>
       <c r="B320" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C320" s="1">
         <v>1.0</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="321">
@@ -6079,13 +6079,13 @@
         <v>332</v>
       </c>
       <c r="B321" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C321" s="1">
         <v>1.0</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="322">
@@ -6093,13 +6093,13 @@
         <v>333</v>
       </c>
       <c r="B322" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C322" s="1">
         <v>1.0</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="323">
@@ -6107,13 +6107,13 @@
         <v>334</v>
       </c>
       <c r="B323" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C323" s="1">
         <v>1.0</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="324">
@@ -6121,13 +6121,13 @@
         <v>335</v>
       </c>
       <c r="B324" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C324" s="1">
         <v>1.0</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="325">
@@ -6135,13 +6135,13 @@
         <v>336</v>
       </c>
       <c r="B325" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C325" s="1">
         <v>1.0</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="326">
@@ -6149,13 +6149,13 @@
         <v>337</v>
       </c>
       <c r="B326" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C326" s="1">
         <v>1.0</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="327">
@@ -6163,13 +6163,13 @@
         <v>338</v>
       </c>
       <c r="B327" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C327" s="1">
         <v>1.0</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="328">
@@ -6177,13 +6177,13 @@
         <v>339</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C328" s="1">
         <v>1.0</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="329">
@@ -6191,13 +6191,13 @@
         <v>340</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C329" s="1">
         <v>1.0</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="330">
@@ -6205,13 +6205,13 @@
         <v>341</v>
       </c>
       <c r="B330" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C330" s="1">
         <v>1.0</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="331">
@@ -6219,13 +6219,13 @@
         <v>342</v>
       </c>
       <c r="B331" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C331" s="1">
         <v>1.0</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="332">
@@ -6233,13 +6233,13 @@
         <v>343</v>
       </c>
       <c r="B332" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C332" s="1">
         <v>1.0</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="333">
@@ -6247,13 +6247,13 @@
         <v>344</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C333" s="1">
         <v>1.0</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="334">
@@ -6261,13 +6261,13 @@
         <v>345</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C334" s="1">
         <v>1.0</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="335">
@@ -6275,10 +6275,13 @@
         <v>346</v>
       </c>
       <c r="B335" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C335" s="1">
-        <v>-1.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="336">
@@ -6286,7 +6289,7 @@
         <v>347</v>
       </c>
       <c r="B336" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C336" s="1">
         <v>-1.0</v>
@@ -6297,7 +6300,7 @@
         <v>348</v>
       </c>
       <c r="B337" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C337" s="1">
         <v>-1.0</v>
@@ -6308,7 +6311,7 @@
         <v>349</v>
       </c>
       <c r="B338" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C338" s="1">
         <v>-1.0</v>
@@ -6319,7 +6322,7 @@
         <v>350</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C339" s="1">
         <v>-1.0</v>
@@ -6330,7 +6333,7 @@
         <v>351</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C340" s="1">
         <v>-1.0</v>
@@ -6341,7 +6344,7 @@
         <v>352</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C341" s="1">
         <v>-1.0</v>
@@ -6349,10 +6352,10 @@
     </row>
     <row r="342">
       <c r="A342" s="1" t="s">
-        <v>45</v>
+        <v>353</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C342" s="1">
         <v>-1.0</v>
@@ -6360,10 +6363,10 @@
     </row>
     <row r="343">
       <c r="A343" s="1" t="s">
-        <v>353</v>
+        <v>45</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C343" s="1">
         <v>-1.0</v>
@@ -6374,7 +6377,7 @@
         <v>354</v>
       </c>
       <c r="B344" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C344" s="1">
         <v>-1.0</v>
@@ -6385,7 +6388,7 @@
         <v>355</v>
       </c>
       <c r="B345" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C345" s="1">
         <v>-1.0</v>
@@ -6396,7 +6399,7 @@
         <v>356</v>
       </c>
       <c r="B346" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C346" s="1">
         <v>-1.0</v>
@@ -6407,7 +6410,7 @@
         <v>357</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C347" s="1">
         <v>-1.0</v>
@@ -6418,7 +6421,7 @@
         <v>358</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C348" s="1">
         <v>-1.0</v>
@@ -6429,7 +6432,7 @@
         <v>359</v>
       </c>
       <c r="B349" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C349" s="1">
         <v>-1.0</v>
@@ -6440,7 +6443,7 @@
         <v>360</v>
       </c>
       <c r="B350" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C350" s="1">
         <v>-1.0</v>
@@ -6451,7 +6454,7 @@
         <v>361</v>
       </c>
       <c r="B351" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C351" s="1">
         <v>-1.0</v>
@@ -6462,7 +6465,7 @@
         <v>362</v>
       </c>
       <c r="B352" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C352" s="1">
         <v>-1.0</v>
@@ -6473,7 +6476,7 @@
         <v>363</v>
       </c>
       <c r="B353" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C353" s="1">
         <v>-1.0</v>
@@ -6484,7 +6487,7 @@
         <v>364</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C354" s="1">
         <v>-1.0</v>
@@ -6495,7 +6498,7 @@
         <v>365</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C355" s="1">
         <v>-1.0</v>
@@ -6506,7 +6509,7 @@
         <v>366</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C356" s="1">
         <v>-1.0</v>
@@ -6517,7 +6520,7 @@
         <v>367</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C357" s="1">
         <v>-1.0</v>
@@ -6528,7 +6531,7 @@
         <v>368</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C358" s="1">
         <v>-1.0</v>
@@ -6539,7 +6542,7 @@
         <v>369</v>
       </c>
       <c r="B359" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C359" s="1">
         <v>-1.0</v>
@@ -6547,10 +6550,10 @@
     </row>
     <row r="360">
       <c r="A360" s="1" t="s">
-        <v>100</v>
+        <v>370</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C360" s="1">
         <v>-1.0</v>
@@ -6558,10 +6561,10 @@
     </row>
     <row r="361">
       <c r="A361" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C361" s="1">
         <v>-1.0</v>
@@ -6569,10 +6572,10 @@
     </row>
     <row r="362">
       <c r="A362" s="1" t="s">
-        <v>370</v>
+        <v>135</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C362" s="1">
         <v>-1.0</v>
@@ -6583,7 +6586,7 @@
         <v>371</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C363" s="1">
         <v>-1.0</v>
@@ -6594,7 +6597,7 @@
         <v>372</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C364" s="1">
         <v>-1.0</v>
@@ -6605,7 +6608,7 @@
         <v>373</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C365" s="1">
         <v>-1.0</v>
@@ -6616,7 +6619,7 @@
         <v>374</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C366" s="1">
         <v>-1.0</v>
@@ -6627,7 +6630,7 @@
         <v>375</v>
       </c>
       <c r="B367" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C367" s="1">
         <v>-1.0</v>
@@ -6638,7 +6641,7 @@
         <v>376</v>
       </c>
       <c r="B368" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C368" s="1">
         <v>-1.0</v>
@@ -6649,7 +6652,7 @@
         <v>377</v>
       </c>
       <c r="B369" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C369" s="1">
         <v>-1.0</v>
@@ -6660,7 +6663,7 @@
         <v>378</v>
       </c>
       <c r="B370" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C370" s="1">
         <v>-1.0</v>
@@ -6671,7 +6674,7 @@
         <v>379</v>
       </c>
       <c r="B371" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C371" s="1">
         <v>-1.0</v>
@@ -6682,7 +6685,7 @@
         <v>380</v>
       </c>
       <c r="B372" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C372" s="1">
         <v>-1.0</v>
@@ -6693,7 +6696,7 @@
         <v>381</v>
       </c>
       <c r="B373" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C373" s="1">
         <v>-1.0</v>
@@ -6704,7 +6707,7 @@
         <v>382</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C374" s="1">
         <v>-1.0</v>
@@ -6715,7 +6718,7 @@
         <v>383</v>
       </c>
       <c r="B375" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C375" s="1">
         <v>-1.0</v>
@@ -6726,7 +6729,7 @@
         <v>384</v>
       </c>
       <c r="B376" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C376" s="1">
         <v>-1.0</v>
@@ -6737,7 +6740,7 @@
         <v>385</v>
       </c>
       <c r="B377" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C377" s="1">
         <v>-1.0</v>
@@ -6748,7 +6751,7 @@
         <v>386</v>
       </c>
       <c r="B378" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C378" s="1">
         <v>-1.0</v>
@@ -6759,7 +6762,7 @@
         <v>387</v>
       </c>
       <c r="B379" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C379" s="1">
         <v>-1.0</v>
@@ -6767,10 +6770,10 @@
     </row>
     <row r="380">
       <c r="A380" s="1" t="s">
-        <v>212</v>
+        <v>388</v>
       </c>
       <c r="B380" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C380" s="1">
         <v>-1.0</v>
@@ -6778,10 +6781,10 @@
     </row>
     <row r="381">
       <c r="A381" s="1" t="s">
-        <v>388</v>
+        <v>212</v>
       </c>
       <c r="B381" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C381" s="1">
         <v>-1.0</v>
@@ -6789,10 +6792,10 @@
     </row>
     <row r="382">
       <c r="A382" s="1" t="s">
-        <v>213</v>
+        <v>389</v>
       </c>
       <c r="B382" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C382" s="1">
         <v>-1.0</v>
@@ -6800,10 +6803,10 @@
     </row>
     <row r="383">
       <c r="A383" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B383" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C383" s="1">
         <v>-1.0</v>
@@ -6811,10 +6814,10 @@
     </row>
     <row r="384">
       <c r="A384" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B384" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C384" s="1">
         <v>-1.0</v>
@@ -6822,10 +6825,10 @@
     </row>
     <row r="385">
       <c r="A385" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B385" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C385" s="1">
         <v>-1.0</v>
@@ -6833,10 +6836,10 @@
     </row>
     <row r="386">
       <c r="A386" s="1" t="s">
-        <v>389</v>
+        <v>216</v>
       </c>
       <c r="B386" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C386" s="1">
         <v>-1.0</v>
@@ -6847,7 +6850,7 @@
         <v>390</v>
       </c>
       <c r="B387" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C387" s="1">
         <v>-1.0</v>
@@ -6858,7 +6861,7 @@
         <v>391</v>
       </c>
       <c r="B388" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C388" s="1">
         <v>-1.0</v>
@@ -6869,7 +6872,7 @@
         <v>392</v>
       </c>
       <c r="B389" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C389" s="1">
         <v>-1.0</v>
@@ -6880,7 +6883,7 @@
         <v>393</v>
       </c>
       <c r="B390" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C390" s="1">
         <v>-1.0</v>
@@ -6891,7 +6894,7 @@
         <v>394</v>
       </c>
       <c r="B391" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C391" s="1">
         <v>-1.0</v>
@@ -6902,7 +6905,7 @@
         <v>395</v>
       </c>
       <c r="B392" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C392" s="1">
         <v>-1.0</v>
@@ -6913,7 +6916,7 @@
         <v>396</v>
       </c>
       <c r="B393" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C393" s="1">
         <v>-1.0</v>
@@ -6924,7 +6927,7 @@
         <v>397</v>
       </c>
       <c r="B394" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C394" s="1">
         <v>-1.0</v>
@@ -6935,7 +6938,7 @@
         <v>398</v>
       </c>
       <c r="B395" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C395" s="1">
         <v>-1.0</v>
@@ -6946,7 +6949,7 @@
         <v>399</v>
       </c>
       <c r="B396" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C396" s="1">
         <v>-1.0</v>
@@ -6957,7 +6960,7 @@
         <v>400</v>
       </c>
       <c r="B397" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C397" s="1">
         <v>-1.0</v>
@@ -6968,7 +6971,7 @@
         <v>401</v>
       </c>
       <c r="B398" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C398" s="1">
         <v>-1.0</v>
@@ -6979,27 +6982,24 @@
         <v>402</v>
       </c>
       <c r="B399" s="1" t="s">
-        <v>403</v>
+        <v>325</v>
       </c>
       <c r="C399" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D399" s="1" t="s">
-        <v>404</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C400" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D400" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="B400" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C400" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D400" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="401">
@@ -7007,13 +7007,13 @@
         <v>406</v>
       </c>
       <c r="B401" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C401" s="1">
         <v>1.0</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="402">
@@ -7021,13 +7021,13 @@
         <v>407</v>
       </c>
       <c r="B402" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C402" s="1">
         <v>1.0</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="403">
@@ -7035,13 +7035,13 @@
         <v>408</v>
       </c>
       <c r="B403" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C403" s="1">
         <v>1.0</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="404">
@@ -7049,13 +7049,13 @@
         <v>409</v>
       </c>
       <c r="B404" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C404" s="1">
         <v>1.0</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="405">
@@ -7063,27 +7063,27 @@
         <v>410</v>
       </c>
       <c r="B405" s="1" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C405" s="1">
         <v>1.0</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C406" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D406" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B406" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C406" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D406" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="407">
@@ -7091,13 +7091,13 @@
         <v>414</v>
       </c>
       <c r="B407" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C407" s="1">
         <v>1.0</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="408">
@@ -7105,13 +7105,13 @@
         <v>415</v>
       </c>
       <c r="B408" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C408" s="1">
         <v>1.0</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="409">
@@ -7119,13 +7119,13 @@
         <v>416</v>
       </c>
       <c r="B409" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C409" s="1">
         <v>1.0</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="410">
@@ -7133,13 +7133,13 @@
         <v>417</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C410" s="1">
         <v>1.0</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="411">
@@ -7147,13 +7147,13 @@
         <v>418</v>
       </c>
       <c r="B411" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C411" s="1">
         <v>1.0</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="412">
@@ -7161,13 +7161,13 @@
         <v>419</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C412" s="1">
         <v>1.0</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="413">
@@ -7175,13 +7175,13 @@
         <v>420</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C413" s="1">
         <v>1.0</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="414">
@@ -7189,13 +7189,13 @@
         <v>421</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C414" s="1">
         <v>1.0</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="415">
@@ -7203,13 +7203,13 @@
         <v>422</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C415" s="1">
         <v>1.0</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="416">
@@ -7217,41 +7217,41 @@
         <v>423</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C416" s="1">
         <v>1.0</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="s">
-        <v>370</v>
+        <v>424</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C417" s="1">
         <v>1.0</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="s">
-        <v>424</v>
+        <v>371</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C418" s="1">
         <v>1.0</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="419">
@@ -7259,13 +7259,13 @@
         <v>425</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C419" s="1">
         <v>1.0</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="420">
@@ -7273,13 +7273,13 @@
         <v>426</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C420" s="1">
         <v>1.0</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="421">
@@ -7287,13 +7287,13 @@
         <v>427</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C421" s="1">
         <v>1.0</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="422">
@@ -7301,13 +7301,13 @@
         <v>428</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C422" s="1">
         <v>1.0</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="423">
@@ -7315,13 +7315,13 @@
         <v>429</v>
       </c>
       <c r="B423" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C423" s="1">
         <v>1.0</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="424">
@@ -7329,13 +7329,13 @@
         <v>430</v>
       </c>
       <c r="B424" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C424" s="1">
         <v>1.0</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="425">
@@ -7343,13 +7343,13 @@
         <v>431</v>
       </c>
       <c r="B425" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C425" s="1">
         <v>1.0</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="426">
@@ -7357,13 +7357,13 @@
         <v>432</v>
       </c>
       <c r="B426" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C426" s="1">
         <v>1.0</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="427">
@@ -7371,13 +7371,13 @@
         <v>433</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C427" s="1">
         <v>1.0</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="428">
@@ -7385,13 +7385,13 @@
         <v>434</v>
       </c>
       <c r="B428" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C428" s="1">
         <v>1.0</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="429">
@@ -7399,13 +7399,13 @@
         <v>435</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C429" s="1">
         <v>1.0</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="430">
@@ -7413,13 +7413,13 @@
         <v>436</v>
       </c>
       <c r="B430" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C430" s="1">
         <v>1.0</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="431">
@@ -7427,13 +7427,13 @@
         <v>437</v>
       </c>
       <c r="B431" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C431" s="1">
         <v>1.0</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="432">
@@ -7441,13 +7441,13 @@
         <v>438</v>
       </c>
       <c r="B432" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C432" s="1">
         <v>1.0</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="433">
@@ -7455,13 +7455,13 @@
         <v>439</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C433" s="1">
         <v>1.0</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="434">
@@ -7469,13 +7469,13 @@
         <v>440</v>
       </c>
       <c r="B434" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C434" s="1">
         <v>1.0</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="435">
@@ -7483,13 +7483,13 @@
         <v>441</v>
       </c>
       <c r="B435" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C435" s="1">
         <v>1.0</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="436">
@@ -7497,13 +7497,13 @@
         <v>442</v>
       </c>
       <c r="B436" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C436" s="1">
         <v>1.0</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="437">
@@ -7511,13 +7511,13 @@
         <v>443</v>
       </c>
       <c r="B437" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C437" s="1">
         <v>1.0</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="438">
@@ -7525,13 +7525,13 @@
         <v>444</v>
       </c>
       <c r="B438" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C438" s="1">
         <v>1.0</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="439">
@@ -7539,13 +7539,13 @@
         <v>445</v>
       </c>
       <c r="B439" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C439" s="1">
         <v>1.0</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="440">
@@ -7553,13 +7553,13 @@
         <v>446</v>
       </c>
       <c r="B440" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C440" s="1">
         <v>1.0</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="441">
@@ -7567,13 +7567,13 @@
         <v>447</v>
       </c>
       <c r="B441" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C441" s="1">
         <v>1.0</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="442">
@@ -7581,13 +7581,13 @@
         <v>448</v>
       </c>
       <c r="B442" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C442" s="1">
         <v>1.0</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="443">
@@ -7595,13 +7595,13 @@
         <v>449</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C443" s="1">
         <v>1.0</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="444">
@@ -7609,13 +7609,13 @@
         <v>450</v>
       </c>
       <c r="B444" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C444" s="1">
         <v>1.0</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="445">
@@ -7623,13 +7623,13 @@
         <v>451</v>
       </c>
       <c r="B445" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C445" s="1">
         <v>1.0</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="446">
@@ -7637,13 +7637,13 @@
         <v>452</v>
       </c>
       <c r="B446" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C446" s="1">
         <v>1.0</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="447">
@@ -7651,13 +7651,13 @@
         <v>453</v>
       </c>
       <c r="B447" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C447" s="1">
         <v>1.0</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="448">
@@ -7665,27 +7665,27 @@
         <v>454</v>
       </c>
       <c r="B448" s="1" t="s">
-        <v>455</v>
+        <v>412</v>
       </c>
       <c r="C448" s="1">
         <v>1.0</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>456</v>
+        <v>413</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C449" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D449" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="B449" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C449" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D449" s="1" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="450">
@@ -7693,13 +7693,13 @@
         <v>458</v>
       </c>
       <c r="B450" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C450" s="1">
         <v>1.0</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="451">
@@ -7707,13 +7707,13 @@
         <v>459</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C451" s="1">
         <v>1.0</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="452">
@@ -7721,13 +7721,13 @@
         <v>460</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C452" s="1">
         <v>1.0</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="453">
@@ -7735,13 +7735,13 @@
         <v>461</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C453" s="1">
         <v>1.0</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="454">
@@ -7749,13 +7749,13 @@
         <v>462</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C454" s="1">
         <v>1.0</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="455">
@@ -7763,27 +7763,27 @@
         <v>463</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="C455" s="1">
         <v>1.0</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C456" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D456" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="B456" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C456" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D456" s="1" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="457">
@@ -7791,13 +7791,13 @@
         <v>467</v>
       </c>
       <c r="B457" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C457" s="1">
         <v>1.0</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="458">
@@ -7805,13 +7805,13 @@
         <v>468</v>
       </c>
       <c r="B458" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C458" s="1">
         <v>1.0</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="459">
@@ -7819,13 +7819,13 @@
         <v>469</v>
       </c>
       <c r="B459" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C459" s="1">
         <v>1.0</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="460">
@@ -7833,13 +7833,13 @@
         <v>470</v>
       </c>
       <c r="B460" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C460" s="1">
         <v>1.0</v>
       </c>
       <c r="D460" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="461">
@@ -7847,27 +7847,27 @@
         <v>471</v>
       </c>
       <c r="B461" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C461" s="1">
         <v>1.0</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C462" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="D462" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="B462" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="C462" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="D462" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="463">
@@ -7875,13 +7875,13 @@
         <v>474</v>
       </c>
       <c r="B463" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C463" s="1">
         <v>1.0</v>
       </c>
       <c r="D463" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="464">
@@ -7889,13 +7889,13 @@
         <v>475</v>
       </c>
       <c r="B464" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C464" s="1">
         <v>1.0</v>
       </c>
       <c r="D464" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="465">
@@ -7903,13 +7903,13 @@
         <v>476</v>
       </c>
       <c r="B465" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C465" s="1">
         <v>1.0</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="466">
@@ -7917,13 +7917,13 @@
         <v>477</v>
       </c>
       <c r="B466" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C466" s="1">
         <v>1.0</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="467">
@@ -7931,13 +7931,13 @@
         <v>478</v>
       </c>
       <c r="B467" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C467" s="1">
         <v>1.0</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="468">
@@ -7945,13 +7945,13 @@
         <v>479</v>
       </c>
       <c r="B468" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C468" s="1">
         <v>1.0</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="469">
@@ -7959,13 +7959,13 @@
         <v>480</v>
       </c>
       <c r="B469" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C469" s="1">
         <v>1.0</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="470">
@@ -7973,13 +7973,13 @@
         <v>481</v>
       </c>
       <c r="B470" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C470" s="1">
         <v>1.0</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="471">
@@ -7987,13 +7987,13 @@
         <v>482</v>
       </c>
       <c r="B471" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C471" s="1">
         <v>1.0</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="472">
@@ -8001,13 +8001,13 @@
         <v>483</v>
       </c>
       <c r="B472" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C472" s="1">
         <v>1.0</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="473">
@@ -8015,13 +8015,13 @@
         <v>484</v>
       </c>
       <c r="B473" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C473" s="1">
         <v>1.0</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="474">
@@ -8029,13 +8029,13 @@
         <v>485</v>
       </c>
       <c r="B474" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C474" s="1">
         <v>1.0</v>
       </c>
       <c r="D474" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="475">
@@ -8043,13 +8043,13 @@
         <v>486</v>
       </c>
       <c r="B475" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C475" s="1">
         <v>1.0</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="476">
@@ -8057,13 +8057,13 @@
         <v>487</v>
       </c>
       <c r="B476" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C476" s="1">
         <v>1.0</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="477">
@@ -8071,13 +8071,13 @@
         <v>488</v>
       </c>
       <c r="B477" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C477" s="1">
         <v>1.0</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="478">
@@ -8085,13 +8085,13 @@
         <v>489</v>
       </c>
       <c r="B478" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C478" s="1">
         <v>1.0</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="479">
@@ -8099,13 +8099,13 @@
         <v>490</v>
       </c>
       <c r="B479" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C479" s="1">
         <v>1.0</v>
       </c>
       <c r="D479" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="480">
@@ -8113,13 +8113,13 @@
         <v>491</v>
       </c>
       <c r="B480" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C480" s="1">
         <v>1.0</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="481">
@@ -8127,13 +8127,13 @@
         <v>492</v>
       </c>
       <c r="B481" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C481" s="1">
         <v>1.0</v>
       </c>
       <c r="D481" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="482">
@@ -8141,13 +8141,13 @@
         <v>493</v>
       </c>
       <c r="B482" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C482" s="1">
         <v>1.0</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="483">
@@ -8155,13 +8155,13 @@
         <v>494</v>
       </c>
       <c r="B483" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C483" s="1">
         <v>1.0</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="484">
@@ -8169,13 +8169,13 @@
         <v>495</v>
       </c>
       <c r="B484" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C484" s="1">
         <v>1.0</v>
       </c>
       <c r="D484" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="485">
@@ -8183,41 +8183,41 @@
         <v>496</v>
       </c>
       <c r="B485" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C485" s="1">
         <v>1.0</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" s="1" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="B486" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C486" s="1">
         <v>1.0</v>
       </c>
       <c r="D486" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B487" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C487" s="1">
         <v>1.0</v>
       </c>
       <c r="D487" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="488">
@@ -8225,13 +8225,13 @@
         <v>498</v>
       </c>
       <c r="B488" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C488" s="1">
         <v>1.0</v>
       </c>
       <c r="D488" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="489">
@@ -8239,13 +8239,13 @@
         <v>499</v>
       </c>
       <c r="B489" s="1" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C489" s="1">
         <v>1.0</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="490">
@@ -8253,18 +8253,21 @@
         <v>500</v>
       </c>
       <c r="B490" s="1" t="s">
-        <v>501</v>
+        <v>465</v>
       </c>
       <c r="C490" s="1">
         <v>1.0</v>
+      </c>
+      <c r="D490" s="1" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B491" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C491" s="1">
         <v>1.0</v>
@@ -8275,7 +8278,7 @@
         <v>503</v>
       </c>
       <c r="B492" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C492" s="1">
         <v>1.0</v>
@@ -8286,7 +8289,7 @@
         <v>504</v>
       </c>
       <c r="B493" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C493" s="1">
         <v>1.0</v>
@@ -8297,7 +8300,7 @@
         <v>505</v>
       </c>
       <c r="B494" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C494" s="1">
         <v>1.0</v>
@@ -8308,7 +8311,7 @@
         <v>506</v>
       </c>
       <c r="B495" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C495" s="1">
         <v>1.0</v>
@@ -8319,7 +8322,7 @@
         <v>507</v>
       </c>
       <c r="B496" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C496" s="1">
         <v>1.0</v>
@@ -8330,7 +8333,7 @@
         <v>508</v>
       </c>
       <c r="B497" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C497" s="1">
         <v>1.0</v>
@@ -8341,7 +8344,7 @@
         <v>509</v>
       </c>
       <c r="B498" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C498" s="1">
         <v>1.0</v>
@@ -8352,7 +8355,7 @@
         <v>510</v>
       </c>
       <c r="B499" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C499" s="1">
         <v>1.0</v>
@@ -8363,7 +8366,7 @@
         <v>511</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C500" s="1">
         <v>1.0</v>
@@ -8374,7 +8377,7 @@
         <v>512</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C501" s="1">
         <v>1.0</v>
@@ -8385,7 +8388,7 @@
         <v>513</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C502" s="1">
         <v>1.0</v>
@@ -8396,7 +8399,7 @@
         <v>514</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C503" s="1">
         <v>1.0</v>
@@ -8407,7 +8410,7 @@
         <v>515</v>
       </c>
       <c r="B504" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C504" s="1">
         <v>1.0</v>
@@ -8418,7 +8421,7 @@
         <v>516</v>
       </c>
       <c r="B505" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C505" s="1">
         <v>1.0</v>
@@ -8429,7 +8432,7 @@
         <v>517</v>
       </c>
       <c r="B506" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C506" s="1">
         <v>1.0</v>
@@ -8440,7 +8443,7 @@
         <v>518</v>
       </c>
       <c r="B507" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C507" s="1">
         <v>1.0</v>
@@ -8451,7 +8454,7 @@
         <v>519</v>
       </c>
       <c r="B508" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C508" s="1">
         <v>1.0</v>
@@ -8462,7 +8465,7 @@
         <v>520</v>
       </c>
       <c r="B509" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C509" s="1">
         <v>1.0</v>
@@ -8473,7 +8476,7 @@
         <v>521</v>
       </c>
       <c r="B510" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C510" s="1">
         <v>1.0</v>
@@ -8484,7 +8487,7 @@
         <v>522</v>
       </c>
       <c r="B511" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C511" s="1">
         <v>1.0</v>
@@ -8495,7 +8498,7 @@
         <v>523</v>
       </c>
       <c r="B512" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C512" s="1">
         <v>1.0</v>
@@ -8506,7 +8509,7 @@
         <v>524</v>
       </c>
       <c r="B513" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C513" s="1">
         <v>1.0</v>
@@ -8517,7 +8520,7 @@
         <v>525</v>
       </c>
       <c r="B514" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C514" s="1">
         <v>1.0</v>
@@ -8528,7 +8531,7 @@
         <v>526</v>
       </c>
       <c r="B515" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C515" s="1">
         <v>1.0</v>
@@ -8539,7 +8542,7 @@
         <v>527</v>
       </c>
       <c r="B516" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C516" s="1">
         <v>1.0</v>
@@ -8550,7 +8553,7 @@
         <v>528</v>
       </c>
       <c r="B517" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C517" s="1">
         <v>1.0</v>
@@ -8561,7 +8564,7 @@
         <v>529</v>
       </c>
       <c r="B518" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C518" s="1">
         <v>1.0</v>
@@ -8572,7 +8575,7 @@
         <v>530</v>
       </c>
       <c r="B519" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C519" s="1">
         <v>1.0</v>
@@ -8583,7 +8586,7 @@
         <v>531</v>
       </c>
       <c r="B520" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C520" s="1">
         <v>1.0</v>
@@ -8594,7 +8597,7 @@
         <v>532</v>
       </c>
       <c r="B521" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C521" s="1">
         <v>1.0</v>
@@ -8605,7 +8608,7 @@
         <v>533</v>
       </c>
       <c r="B522" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C522" s="1">
         <v>1.0</v>
@@ -8616,7 +8619,7 @@
         <v>534</v>
       </c>
       <c r="B523" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C523" s="1">
         <v>1.0</v>
@@ -8627,7 +8630,7 @@
         <v>535</v>
       </c>
       <c r="B524" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C524" s="1">
         <v>1.0</v>
@@ -8638,7 +8641,7 @@
         <v>536</v>
       </c>
       <c r="B525" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C525" s="1">
         <v>1.0</v>
@@ -8649,7 +8652,7 @@
         <v>537</v>
       </c>
       <c r="B526" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C526" s="1">
         <v>1.0</v>
@@ -8660,7 +8663,7 @@
         <v>538</v>
       </c>
       <c r="B527" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C527" s="1">
         <v>1.0</v>
@@ -8671,7 +8674,7 @@
         <v>539</v>
       </c>
       <c r="B528" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C528" s="1">
         <v>1.0</v>
@@ -8682,7 +8685,7 @@
         <v>540</v>
       </c>
       <c r="B529" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C529" s="1">
         <v>1.0</v>
@@ -8693,7 +8696,7 @@
         <v>541</v>
       </c>
       <c r="B530" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C530" s="1">
         <v>1.0</v>
@@ -8704,7 +8707,7 @@
         <v>542</v>
       </c>
       <c r="B531" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C531" s="1">
         <v>1.0</v>
@@ -8715,7 +8718,7 @@
         <v>543</v>
       </c>
       <c r="B532" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C532" s="1">
         <v>1.0</v>
@@ -8726,7 +8729,7 @@
         <v>544</v>
       </c>
       <c r="B533" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C533" s="1">
         <v>1.0</v>
@@ -8737,7 +8740,7 @@
         <v>545</v>
       </c>
       <c r="B534" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C534" s="1">
         <v>1.0</v>
@@ -8748,7 +8751,7 @@
         <v>546</v>
       </c>
       <c r="B535" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C535" s="1">
         <v>1.0</v>
@@ -8759,7 +8762,7 @@
         <v>547</v>
       </c>
       <c r="B536" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C536" s="1">
         <v>1.0</v>
@@ -8770,7 +8773,7 @@
         <v>548</v>
       </c>
       <c r="B537" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C537" s="1">
         <v>1.0</v>
@@ -8781,7 +8784,7 @@
         <v>549</v>
       </c>
       <c r="B538" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C538" s="1">
         <v>1.0</v>
@@ -8792,7 +8795,7 @@
         <v>550</v>
       </c>
       <c r="B539" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C539" s="1">
         <v>1.0</v>
@@ -8803,7 +8806,7 @@
         <v>551</v>
       </c>
       <c r="B540" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C540" s="1">
         <v>1.0</v>
@@ -8814,7 +8817,7 @@
         <v>552</v>
       </c>
       <c r="B541" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C541" s="1">
         <v>1.0</v>
@@ -8825,7 +8828,7 @@
         <v>553</v>
       </c>
       <c r="B542" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C542" s="1">
         <v>1.0</v>
@@ -8836,7 +8839,7 @@
         <v>554</v>
       </c>
       <c r="B543" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C543" s="1">
         <v>1.0</v>
@@ -8847,7 +8850,7 @@
         <v>555</v>
       </c>
       <c r="B544" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C544" s="1">
         <v>1.0</v>
@@ -8858,7 +8861,7 @@
         <v>556</v>
       </c>
       <c r="B545" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C545" s="1">
         <v>1.0</v>
@@ -8869,7 +8872,7 @@
         <v>557</v>
       </c>
       <c r="B546" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C546" s="1">
         <v>1.0</v>
@@ -8880,7 +8883,7 @@
         <v>558</v>
       </c>
       <c r="B547" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C547" s="1">
         <v>1.0</v>
@@ -8891,7 +8894,7 @@
         <v>559</v>
       </c>
       <c r="B548" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C548" s="1">
         <v>1.0</v>
@@ -8902,7 +8905,7 @@
         <v>560</v>
       </c>
       <c r="B549" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C549" s="1">
         <v>1.0</v>
@@ -8913,7 +8916,7 @@
         <v>561</v>
       </c>
       <c r="B550" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C550" s="1">
         <v>1.0</v>
@@ -8924,7 +8927,7 @@
         <v>562</v>
       </c>
       <c r="B551" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C551" s="1">
         <v>1.0</v>
@@ -8935,7 +8938,7 @@
         <v>563</v>
       </c>
       <c r="B552" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C552" s="1">
         <v>1.0</v>
@@ -8946,7 +8949,7 @@
         <v>564</v>
       </c>
       <c r="B553" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C553" s="1">
         <v>1.0</v>
@@ -8957,7 +8960,7 @@
         <v>565</v>
       </c>
       <c r="B554" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C554" s="1">
         <v>1.0</v>
@@ -8968,7 +8971,7 @@
         <v>566</v>
       </c>
       <c r="B555" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C555" s="1">
         <v>1.0</v>
@@ -8979,7 +8982,7 @@
         <v>567</v>
       </c>
       <c r="B556" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C556" s="1">
         <v>1.0</v>
@@ -8990,7 +8993,7 @@
         <v>568</v>
       </c>
       <c r="B557" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C557" s="1">
         <v>1.0</v>
@@ -9001,7 +9004,7 @@
         <v>569</v>
       </c>
       <c r="B558" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C558" s="1">
         <v>1.0</v>
@@ -9012,7 +9015,7 @@
         <v>570</v>
       </c>
       <c r="B559" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C559" s="1">
         <v>1.0</v>
@@ -9023,7 +9026,7 @@
         <v>571</v>
       </c>
       <c r="B560" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C560" s="1">
         <v>1.0</v>
@@ -9034,7 +9037,7 @@
         <v>572</v>
       </c>
       <c r="B561" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C561" s="1">
         <v>1.0</v>
@@ -9045,7 +9048,7 @@
         <v>573</v>
       </c>
       <c r="B562" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C562" s="1">
         <v>1.0</v>
@@ -9056,7 +9059,7 @@
         <v>574</v>
       </c>
       <c r="B563" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C563" s="1">
         <v>1.0</v>
@@ -9067,7 +9070,7 @@
         <v>575</v>
       </c>
       <c r="B564" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C564" s="1">
         <v>1.0</v>
@@ -9078,7 +9081,7 @@
         <v>576</v>
       </c>
       <c r="B565" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C565" s="1">
         <v>1.0</v>
@@ -9089,7 +9092,7 @@
         <v>577</v>
       </c>
       <c r="B566" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C566" s="1">
         <v>1.0</v>
@@ -9100,7 +9103,7 @@
         <v>578</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C567" s="1">
         <v>1.0</v>
@@ -9111,7 +9114,7 @@
         <v>579</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C568" s="1">
         <v>1.0</v>
@@ -9122,7 +9125,7 @@
         <v>580</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C569" s="1">
         <v>1.0</v>
@@ -9133,7 +9136,7 @@
         <v>581</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C570" s="1">
         <v>1.0</v>
@@ -9144,7 +9147,7 @@
         <v>582</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C571" s="1">
         <v>1.0</v>
@@ -9155,7 +9158,7 @@
         <v>583</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C572" s="1">
         <v>1.0</v>
@@ -9166,7 +9169,7 @@
         <v>584</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C573" s="1">
         <v>1.0</v>
@@ -9177,7 +9180,7 @@
         <v>585</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C574" s="1">
         <v>1.0</v>
@@ -9188,7 +9191,7 @@
         <v>586</v>
       </c>
       <c r="B575" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C575" s="1">
         <v>1.0</v>
@@ -9199,7 +9202,7 @@
         <v>587</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C576" s="1">
         <v>1.0</v>
@@ -9210,7 +9213,7 @@
         <v>588</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C577" s="1">
         <v>1.0</v>
@@ -9221,7 +9224,7 @@
         <v>589</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C578" s="1">
         <v>1.0</v>
@@ -9232,7 +9235,7 @@
         <v>590</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C579" s="1">
         <v>1.0</v>
@@ -9243,7 +9246,7 @@
         <v>591</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C580" s="1">
         <v>1.0</v>
@@ -9254,7 +9257,7 @@
         <v>592</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C581" s="1">
         <v>1.0</v>
@@ -9265,7 +9268,7 @@
         <v>593</v>
       </c>
       <c r="B582" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C582" s="1">
         <v>1.0</v>
@@ -9276,7 +9279,7 @@
         <v>594</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C583" s="1">
         <v>1.0</v>
@@ -9287,7 +9290,7 @@
         <v>595</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C584" s="1">
         <v>1.0</v>
@@ -9298,7 +9301,7 @@
         <v>596</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C585" s="1">
         <v>1.0</v>
@@ -9309,7 +9312,7 @@
         <v>597</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C586" s="1">
         <v>1.0</v>
@@ -9320,7 +9323,7 @@
         <v>598</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C587" s="1">
         <v>1.0</v>
@@ -9331,7 +9334,7 @@
         <v>599</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C588" s="1">
         <v>1.0</v>
@@ -9342,7 +9345,7 @@
         <v>600</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C589" s="1">
         <v>1.0</v>
@@ -9353,7 +9356,7 @@
         <v>601</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C590" s="1">
         <v>1.0</v>
@@ -9364,7 +9367,7 @@
         <v>602</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C591" s="1">
         <v>1.0</v>
@@ -9375,7 +9378,7 @@
         <v>603</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C592" s="1">
         <v>1.0</v>
@@ -9386,7 +9389,7 @@
         <v>604</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C593" s="1">
         <v>1.0</v>
@@ -9397,7 +9400,7 @@
         <v>605</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C594" s="1">
         <v>1.0</v>
@@ -9408,7 +9411,7 @@
         <v>606</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C595" s="1">
         <v>1.0</v>
@@ -9419,7 +9422,7 @@
         <v>607</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C596" s="1">
         <v>1.0</v>
@@ -9430,7 +9433,7 @@
         <v>608</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C597" s="1">
         <v>1.0</v>
@@ -9441,7 +9444,7 @@
         <v>609</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C598" s="1">
         <v>1.0</v>
@@ -9452,7 +9455,7 @@
         <v>610</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C599" s="1">
         <v>1.0</v>
@@ -9463,7 +9466,7 @@
         <v>611</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C600" s="1">
         <v>1.0</v>
@@ -9474,7 +9477,7 @@
         <v>612</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C601" s="1">
         <v>1.0</v>
@@ -9485,7 +9488,7 @@
         <v>613</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C602" s="1">
         <v>1.0</v>
@@ -9496,7 +9499,7 @@
         <v>614</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C603" s="1">
         <v>1.0</v>
@@ -9507,7 +9510,7 @@
         <v>615</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C604" s="1">
         <v>1.0</v>
@@ -9518,7 +9521,7 @@
         <v>616</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C605" s="1">
         <v>1.0</v>
@@ -9529,7 +9532,7 @@
         <v>617</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C606" s="1">
         <v>1.0</v>
@@ -9540,7 +9543,7 @@
         <v>618</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C607" s="1">
         <v>1.0</v>
@@ -9551,7 +9554,7 @@
         <v>619</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C608" s="1">
         <v>1.0</v>
@@ -9562,7 +9565,7 @@
         <v>620</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C609" s="1">
         <v>1.0</v>
@@ -9573,7 +9576,7 @@
         <v>621</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C610" s="1">
         <v>1.0</v>
@@ -9584,7 +9587,7 @@
         <v>622</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C611" s="1">
         <v>1.0</v>
@@ -9595,7 +9598,7 @@
         <v>623</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C612" s="1">
         <v>1.0</v>
@@ -9606,7 +9609,7 @@
         <v>624</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C613" s="1">
         <v>1.0</v>
@@ -9617,7 +9620,7 @@
         <v>625</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C614" s="1">
         <v>1.0</v>
@@ -9628,7 +9631,7 @@
         <v>626</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C615" s="1">
         <v>1.0</v>
@@ -9639,7 +9642,7 @@
         <v>627</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C616" s="1">
         <v>1.0</v>
@@ -9650,7 +9653,7 @@
         <v>628</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C617" s="1">
         <v>1.0</v>
@@ -9661,7 +9664,7 @@
         <v>629</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C618" s="1">
         <v>1.0</v>
@@ -9672,7 +9675,7 @@
         <v>630</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C619" s="1">
         <v>1.0</v>
@@ -9683,7 +9686,7 @@
         <v>631</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C620" s="1">
         <v>1.0</v>
@@ -9694,7 +9697,7 @@
         <v>632</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C621" s="1">
         <v>1.0</v>
@@ -9705,7 +9708,7 @@
         <v>633</v>
       </c>
       <c r="B622" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C622" s="1">
         <v>1.0</v>
@@ -9716,7 +9719,7 @@
         <v>634</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C623" s="1">
         <v>1.0</v>
@@ -9727,7 +9730,7 @@
         <v>635</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C624" s="1">
         <v>1.0</v>
@@ -9738,7 +9741,7 @@
         <v>636</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C625" s="1">
         <v>1.0</v>
@@ -9749,7 +9752,7 @@
         <v>637</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C626" s="1">
         <v>1.0</v>
@@ -9760,7 +9763,7 @@
         <v>638</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C627" s="1">
         <v>1.0</v>
@@ -9771,7 +9774,7 @@
         <v>639</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C628" s="1">
         <v>1.0</v>
@@ -9782,7 +9785,7 @@
         <v>640</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C629" s="1">
         <v>1.0</v>
@@ -9793,7 +9796,7 @@
         <v>641</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C630" s="1">
         <v>1.0</v>
@@ -9804,7 +9807,7 @@
         <v>642</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C631" s="1">
         <v>1.0</v>
@@ -9815,7 +9818,7 @@
         <v>643</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C632" s="1">
         <v>1.0</v>
@@ -9826,7 +9829,7 @@
         <v>644</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C633" s="1">
         <v>1.0</v>
@@ -9837,7 +9840,7 @@
         <v>645</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C634" s="1">
         <v>1.0</v>
@@ -9848,7 +9851,7 @@
         <v>646</v>
       </c>
       <c r="B635" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C635" s="1">
         <v>1.0</v>
@@ -9859,7 +9862,7 @@
         <v>647</v>
       </c>
       <c r="B636" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C636" s="1">
         <v>1.0</v>
@@ -9870,7 +9873,7 @@
         <v>648</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C637" s="1">
         <v>1.0</v>
@@ -9881,7 +9884,7 @@
         <v>649</v>
       </c>
       <c r="B638" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C638" s="1">
         <v>1.0</v>
@@ -9892,7 +9895,7 @@
         <v>650</v>
       </c>
       <c r="B639" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C639" s="1">
         <v>1.0</v>
@@ -9903,7 +9906,7 @@
         <v>651</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C640" s="1">
         <v>1.0</v>
@@ -9914,7 +9917,7 @@
         <v>652</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C641" s="1">
         <v>1.0</v>
@@ -9925,7 +9928,7 @@
         <v>653</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C642" s="1">
         <v>1.0</v>
@@ -9936,7 +9939,7 @@
         <v>654</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C643" s="1">
         <v>1.0</v>
@@ -9947,7 +9950,7 @@
         <v>655</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C644" s="1">
         <v>1.0</v>
@@ -9958,7 +9961,7 @@
         <v>656</v>
       </c>
       <c r="B645" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C645" s="1">
         <v>1.0</v>
@@ -9969,7 +9972,7 @@
         <v>657</v>
       </c>
       <c r="B646" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C646" s="1">
         <v>1.0</v>
@@ -9980,7 +9983,7 @@
         <v>658</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C647" s="1">
         <v>1.0</v>
@@ -9991,7 +9994,7 @@
         <v>659</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C648" s="1">
         <v>1.0</v>
@@ -10002,7 +10005,7 @@
         <v>660</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C649" s="1">
         <v>1.0</v>
@@ -10013,7 +10016,7 @@
         <v>661</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C650" s="1">
         <v>1.0</v>
@@ -10024,7 +10027,7 @@
         <v>662</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C651" s="1">
         <v>1.0</v>
@@ -10035,7 +10038,7 @@
         <v>663</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C652" s="1">
         <v>1.0</v>
@@ -10046,7 +10049,7 @@
         <v>664</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C653" s="1">
         <v>1.0</v>
@@ -10057,7 +10060,7 @@
         <v>665</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C654" s="1">
         <v>1.0</v>
@@ -10068,7 +10071,7 @@
         <v>666</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C655" s="1">
         <v>1.0</v>
@@ -10079,7 +10082,7 @@
         <v>667</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C656" s="1">
         <v>1.0</v>
@@ -10090,7 +10093,7 @@
         <v>668</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C657" s="1">
         <v>1.0</v>
@@ -10101,7 +10104,7 @@
         <v>669</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C658" s="1">
         <v>1.0</v>
@@ -10112,7 +10115,7 @@
         <v>670</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C659" s="1">
         <v>1.0</v>
@@ -10123,7 +10126,7 @@
         <v>671</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C660" s="1">
         <v>1.0</v>
@@ -10134,7 +10137,7 @@
         <v>672</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C661" s="1">
         <v>1.0</v>
@@ -10145,7 +10148,7 @@
         <v>673</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C662" s="1">
         <v>1.0</v>
@@ -10156,7 +10159,7 @@
         <v>674</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C663" s="1">
         <v>1.0</v>
@@ -10167,7 +10170,7 @@
         <v>675</v>
       </c>
       <c r="B664" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C664" s="1">
         <v>1.0</v>
@@ -10178,7 +10181,7 @@
         <v>676</v>
       </c>
       <c r="B665" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C665" s="1">
         <v>1.0</v>
@@ -10189,7 +10192,7 @@
         <v>677</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C666" s="1">
         <v>1.0</v>
@@ -10200,7 +10203,7 @@
         <v>678</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C667" s="1">
         <v>1.0</v>
@@ -10211,7 +10214,7 @@
         <v>679</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C668" s="1">
         <v>1.0</v>
@@ -10222,7 +10225,7 @@
         <v>680</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C669" s="1">
         <v>1.0</v>
@@ -10233,7 +10236,7 @@
         <v>681</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C670" s="1">
         <v>1.0</v>
@@ -10244,7 +10247,7 @@
         <v>682</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C671" s="1">
         <v>1.0</v>
@@ -10255,7 +10258,7 @@
         <v>683</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C672" s="1">
         <v>1.0</v>
@@ -10266,7 +10269,7 @@
         <v>684</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C673" s="1">
         <v>1.0</v>
@@ -10277,7 +10280,7 @@
         <v>685</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C674" s="1">
         <v>1.0</v>
@@ -10288,7 +10291,7 @@
         <v>686</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C675" s="1">
         <v>1.0</v>
@@ -10299,7 +10302,7 @@
         <v>687</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C676" s="1">
         <v>1.0</v>
@@ -10310,7 +10313,7 @@
         <v>688</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C677" s="1">
         <v>1.0</v>
@@ -10321,7 +10324,7 @@
         <v>689</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C678" s="1">
         <v>1.0</v>
@@ -10332,7 +10335,7 @@
         <v>690</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C679" s="1">
         <v>1.0</v>
@@ -10343,7 +10346,7 @@
         <v>691</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C680" s="1">
         <v>1.0</v>
@@ -10354,7 +10357,7 @@
         <v>692</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C681" s="1">
         <v>1.0</v>
@@ -10365,7 +10368,7 @@
         <v>693</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C682" s="1">
         <v>1.0</v>
@@ -10376,7 +10379,7 @@
         <v>694</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C683" s="1">
         <v>1.0</v>
@@ -10387,7 +10390,7 @@
         <v>695</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C684" s="1">
         <v>1.0</v>
@@ -10398,7 +10401,7 @@
         <v>696</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C685" s="1">
         <v>1.0</v>
@@ -10409,7 +10412,7 @@
         <v>697</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C686" s="1">
         <v>1.0</v>
@@ -10420,7 +10423,7 @@
         <v>698</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C687" s="1">
         <v>1.0</v>
@@ -10431,7 +10434,7 @@
         <v>699</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C688" s="1">
         <v>1.0</v>
@@ -10442,7 +10445,7 @@
         <v>700</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C689" s="1">
         <v>1.0</v>
@@ -10453,7 +10456,7 @@
         <v>701</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C690" s="1">
         <v>1.0</v>
@@ -10464,7 +10467,7 @@
         <v>702</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C691" s="1">
         <v>1.0</v>
@@ -10475,7 +10478,7 @@
         <v>703</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C692" s="1">
         <v>1.0</v>
@@ -10486,7 +10489,7 @@
         <v>704</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C693" s="1">
         <v>1.0</v>
@@ -10497,7 +10500,7 @@
         <v>705</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C694" s="1">
         <v>1.0</v>
@@ -10508,7 +10511,7 @@
         <v>706</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C695" s="1">
         <v>1.0</v>
@@ -10519,7 +10522,7 @@
         <v>707</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C696" s="1">
         <v>1.0</v>
@@ -10530,7 +10533,7 @@
         <v>708</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C697" s="1">
         <v>1.0</v>
@@ -10541,7 +10544,7 @@
         <v>709</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C698" s="1">
         <v>1.0</v>
@@ -10552,7 +10555,7 @@
         <v>710</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C699" s="1">
         <v>1.0</v>
@@ -10563,7 +10566,7 @@
         <v>711</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C700" s="1">
         <v>1.0</v>
@@ -10574,7 +10577,7 @@
         <v>712</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C701" s="1">
         <v>1.0</v>
@@ -10585,7 +10588,7 @@
         <v>713</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C702" s="1">
         <v>1.0</v>
@@ -10596,7 +10599,7 @@
         <v>714</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C703" s="1">
         <v>1.0</v>
@@ -10607,7 +10610,7 @@
         <v>715</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C704" s="1">
         <v>1.0</v>
@@ -10618,7 +10621,7 @@
         <v>716</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C705" s="1">
         <v>1.0</v>
@@ -10629,7 +10632,7 @@
         <v>717</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C706" s="1">
         <v>1.0</v>
@@ -10640,7 +10643,7 @@
         <v>718</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C707" s="1">
         <v>1.0</v>
@@ -10651,7 +10654,7 @@
         <v>719</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C708" s="1">
         <v>1.0</v>
@@ -10662,7 +10665,7 @@
         <v>720</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C709" s="1">
         <v>1.0</v>
@@ -10673,7 +10676,7 @@
         <v>721</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C710" s="1">
         <v>1.0</v>
@@ -10684,7 +10687,7 @@
         <v>722</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C711" s="1">
         <v>1.0</v>
@@ -10695,7 +10698,7 @@
         <v>723</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C712" s="1">
         <v>1.0</v>
@@ -10706,7 +10709,7 @@
         <v>724</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C713" s="1">
         <v>1.0</v>
@@ -10717,7 +10720,7 @@
         <v>725</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C714" s="1">
         <v>1.0</v>
@@ -10728,7 +10731,7 @@
         <v>726</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C715" s="1">
         <v>1.0</v>
@@ -10739,7 +10742,7 @@
         <v>727</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C716" s="1">
         <v>1.0</v>
@@ -10750,7 +10753,7 @@
         <v>728</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C717" s="1">
         <v>1.0</v>
@@ -10761,7 +10764,7 @@
         <v>729</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C718" s="1">
         <v>1.0</v>
@@ -10772,7 +10775,7 @@
         <v>730</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C719" s="1">
         <v>1.0</v>
@@ -10783,7 +10786,7 @@
         <v>731</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C720" s="1">
         <v>1.0</v>
@@ -10794,7 +10797,7 @@
         <v>732</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C721" s="1">
         <v>1.0</v>
@@ -10805,7 +10808,7 @@
         <v>733</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C722" s="1">
         <v>1.0</v>
@@ -10816,7 +10819,7 @@
         <v>734</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C723" s="1">
         <v>1.0</v>
@@ -10827,7 +10830,7 @@
         <v>735</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C724" s="1">
         <v>1.0</v>
@@ -10838,7 +10841,7 @@
         <v>736</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C725" s="1">
         <v>1.0</v>
@@ -10849,7 +10852,7 @@
         <v>737</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C726" s="1">
         <v>1.0</v>
@@ -10860,7 +10863,7 @@
         <v>738</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C727" s="1">
         <v>1.0</v>
@@ -10871,7 +10874,7 @@
         <v>739</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C728" s="1">
         <v>1.0</v>
@@ -10882,7 +10885,7 @@
         <v>740</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C729" s="1">
         <v>1.0</v>
@@ -10893,7 +10896,7 @@
         <v>741</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C730" s="1">
         <v>1.0</v>
@@ -10904,7 +10907,7 @@
         <v>742</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C731" s="1">
         <v>1.0</v>
@@ -10915,7 +10918,7 @@
         <v>743</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C732" s="1">
         <v>1.0</v>
@@ -10923,10 +10926,10 @@
     </row>
     <row r="733">
       <c r="A733" s="1" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C733" s="1">
         <v>1.0</v>
@@ -10937,7 +10940,7 @@
         <v>742</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C734" s="1">
         <v>1.0</v>
@@ -10948,7 +10951,7 @@
         <v>743</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C735" s="1">
         <v>1.0</v>
@@ -10959,7 +10962,7 @@
         <v>744</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C736" s="1">
         <v>1.0</v>
@@ -10970,7 +10973,7 @@
         <v>745</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C737" s="1">
         <v>1.0</v>
@@ -10981,7 +10984,7 @@
         <v>746</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C738" s="1">
         <v>1.0</v>
@@ -10992,7 +10995,7 @@
         <v>747</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C739" s="1">
         <v>1.0</v>
@@ -11003,7 +11006,7 @@
         <v>748</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C740" s="1">
         <v>1.0</v>
@@ -11014,7 +11017,7 @@
         <v>749</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C741" s="1">
         <v>1.0</v>
@@ -11025,7 +11028,7 @@
         <v>750</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C742" s="1">
         <v>1.0</v>
@@ -11033,10 +11036,10 @@
     </row>
     <row r="743">
       <c r="A743" s="1" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C743" s="1">
         <v>1.0</v>
@@ -11047,7 +11050,7 @@
         <v>749</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C744" s="1">
         <v>1.0</v>
@@ -11058,7 +11061,7 @@
         <v>750</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C745" s="1">
         <v>1.0</v>
@@ -11066,10 +11069,10 @@
     </row>
     <row r="746">
       <c r="A746" s="1" t="s">
-        <v>400</v>
+        <v>751</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C746" s="1">
         <v>1.0</v>
@@ -11077,10 +11080,10 @@
     </row>
     <row r="747">
       <c r="A747" s="1" t="s">
-        <v>751</v>
+        <v>401</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C747" s="1">
         <v>1.0</v>
@@ -11091,9 +11094,20 @@
         <v>752</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C748" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B749" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C749" s="1">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>